<commit_message>
Update IP - EX 39 - Super exercicio I (Anexo).xlsx
Exercicio
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 39 - Super exercicio I (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 39 - Super exercicio I (Anexo).xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8F9E7E-29FE-4E48-A9D3-34C2264D87EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4789565-3A8A-4B50-A5E9-B737EF01B6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
-    <sheet name="EX1-Resolvido" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="EX1-Resolvido" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="anscount" hidden="1">2</definedName>
@@ -35,6 +35,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,7 +673,7 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -793,6 +815,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1294,14 +1324,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:R26"/>
+  <dimension ref="B1:R40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1465,7 +1497,7 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="43">
-        <v>34810</v>
+        <v>35105</v>
       </c>
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
@@ -1515,7 +1547,16 @@
       <c r="Q19" s="13"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="49"/>
+      <c r="B20" s="49" t="str" cm="1">
+        <f t="array" aca="1" ref="B20" ca="1">_xlfn.IFS(TODAY()=$B$16,$L$19,
+MONTH(TODAY())&lt;MONTH($B$16),$L$18,
+MONTH(TODAY())&gt;MONTH($B$16),$L$17,
+MONTH(TODAY())=MONTH($B$16),
+IF((DAY(TODAY())&lt;DAY($B$16)),$L$18,
+IF((DAY(TODAY())&gt;DAY($B$16)),$L$17,$L$19)
+))</f>
+        <v>O funcionário já fez aniversário este ano</v>
+      </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
@@ -1593,6 +1634,66 @@
       <c r="P26" s="25"/>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="66"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="68"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="68"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="68"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C32" s="68"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="68"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="68"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="68"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="68"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="68"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="68"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="68"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>